<commit_message>
update PHO_TableauDeSynthese.xlsx with new data
</commit_message>
<xml_diff>
--- a/public/PHO_TableauDeSynthese.xlsx
+++ b/public/PHO_TableauDeSynthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6D749C-F024-49E9-B794-A12E62FA2A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6513E89-31F6-4EF8-9B0C-32D6066D84D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,7 +152,7 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : https://portfolio-pierre-version-cba.vercel.app</t>
+    <t>Adresse URL du portfolio : https://portfolio-pho-bts.vercel.app</t>
   </si>
 </sst>
 </file>
@@ -667,6 +667,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -678,33 +701,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,8 +925,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -938,56 +938,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="32" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="33"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="41" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="37"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -999,22 +999,22 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="37" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1037,8 +1037,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="324.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1059,16 +1059,16 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
     </row>
     <row r="9" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
@@ -1233,16 +1233,16 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
@@ -1315,16 +1315,16 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="41"/>
     </row>
     <row r="28" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
@@ -11058,6 +11058,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A27:H27"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="A1:F1"/>
@@ -11065,11 +11070,6 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>